<commit_message>
optimize code, delete unused modules, fixed adaptive design, all added preloader instead text
</commit_message>
<xml_diff>
--- a/actions dev.xlsx
+++ b/actions dev.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Везде вместо "Подождите, идет загрузка", поставить прелоадер. Но чтобы не было несколько прелоадеров друг над другом</t>
   </si>
@@ -73,6 +73,27 @@
   </si>
   <si>
     <t>Реализовать добавление в избранное</t>
+  </si>
+  <si>
+    <t>Зайти в 1 курс, перейти в другой курс, отображается урок предыдущего курса</t>
+  </si>
+  <si>
+    <t>Удалить неиспользуемые imports</t>
+  </si>
+  <si>
+    <t>Удалить history и qs библиотеки</t>
+  </si>
+  <si>
+    <t>Увеличить количество разрешенных запросов до 100 в течении 1 мин и блокировкой на 15 сек</t>
+  </si>
+  <si>
+    <t>Исправить желтые подчеркивания</t>
+  </si>
+  <si>
+    <t>Комментарий</t>
+  </si>
+  <si>
+    <t>Нет функционала api</t>
   </si>
 </sst>
 </file>
@@ -142,14 +163,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:B17" totalsRowShown="0">
-  <autoFilter ref="A1:B17"/>
-  <sortState ref="A2:B17">
-    <sortCondition descending="1" ref="B1:B17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:C22" totalsRowShown="0">
+  <autoFilter ref="A1:C22"/>
+  <sortState ref="A2:B22">
+    <sortCondition descending="1" ref="B1:B22"/>
   </sortState>
-  <tableColumns count="2">
+  <tableColumns count="3">
     <tableColumn id="1" name="Что сделать"/>
     <tableColumn id="2" name="Приоритет"/>
+    <tableColumn id="3" name="Комментарий"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -418,151 +440,201 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="158.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B7" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B8" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B9" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B10" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
+      <c r="B11" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="B12" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="B11">
+      <c r="B13">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B12">
+      <c r="B14" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>1</v>
       </c>
-      <c r="B13">
+      <c r="B15">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="1">
         <v>4</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>13</v>
       </c>
-      <c r="B17">
+      <c r="B21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added more pages: detail page course, page content, page matreials and page review. added functional send reviews after completion course
</commit_message>
<xml_diff>
--- a/actions dev.xlsx
+++ b/actions dev.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Везде вместо "Подождите, идет загрузка", поставить прелоадер. Но чтобы не было несколько прелоадеров друг над другом</t>
   </si>
@@ -97,19 +97,51 @@
   </si>
   <si>
     <t>Не пофиксил, но пресек возможные ошибки</t>
+  </si>
+  <si>
+    <t>Отправка отзывов</t>
+  </si>
+  <si>
+    <t>experts вывести, жду когда илья сделает</t>
+  </si>
+  <si>
+    <t> /courses/detail/{id}/reviews  num вывести. Жду,когда илья сделает</t>
+  </si>
+  <si>
+    <t>Функционал написать отзыв</t>
+  </si>
+  <si>
+    <t>/courses/{id}/modules/{id}/lessons вывеси materials</t>
+  </si>
+  <si>
+    <t>Количество записалось на курс в отзывфх</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="5">
@@ -150,11 +182,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -173,10 +207,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:C22" totalsRowShown="0">
-  <autoFilter ref="A1:C22"/>
-  <sortState ref="A2:B22">
-    <sortCondition descending="1" ref="B1:B22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:C28" totalsRowShown="0">
+  <autoFilter ref="A1:C28"/>
+  <sortState ref="A2:C23">
+    <sortCondition descending="1" ref="B1:B23"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="Что сделать"/>
@@ -450,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,10 +509,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>15</v>
       </c>
     </row>
@@ -514,20 +548,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>24</v>
+    <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2">
         <v>9</v>
@@ -537,16 +568,19 @@
       </c>
     </row>
     <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1">
-        <v>8</v>
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1">
         <v>8</v>
@@ -554,107 +588,149 @@
     </row>
     <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B13" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>5</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="C14"/>
+    </row>
+    <row r="15" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B15" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B16" s="3">
         <v>4</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B17" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="C18"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B19" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>12</v>
-      </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>22</v>
       </c>
       <c r="B20">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21"/>
+    </row>
+    <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B21" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="B22" s="1">
         <v>2</v>
       </c>
     </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>